<commit_message>
Added all contracts validations and most sub-recip as well.
</commit_message>
<xml_diff>
--- a/src/server/data/OMB-002-06302020-empty_template-v2.xlsx
+++ b/src/server/data/OMB-002-06302020-empty_template-v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnmclaughlin/git/usdr/cares-reporter/src/server/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B77B6E-41A8-EF4C-9963-79746E65AB23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0787F289-4E95-BE45-A027-995CCE048DEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="-20660" windowWidth="25600" windowHeight="15040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="-20660" windowWidth="25600" windowHeight="15040" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Direct" sheetId="8" r:id="rId8"/>
     <sheet name="Aggregate Awards &lt; 50000" sheetId="9" r:id="rId9"/>
     <sheet name="Aggregate Payments Individual" sheetId="10" r:id="rId10"/>
+    <sheet name="Dropdowns" sheetId="14" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="AgencyCode">Cover!$A:$A</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="230">
   <si>
     <t>Agency Code</t>
   </si>
@@ -376,6 +377,363 @@
   <si>
     <t>Year end</t>
   </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>Projects</t>
+  </si>
+  <si>
+    <t>Subrecipient</t>
+  </si>
+  <si>
+    <t>Multiple</t>
+  </si>
+  <si>
+    <t>Contracts</t>
+  </si>
+  <si>
+    <t>Multiple varies by State</t>
+  </si>
+  <si>
+    <t>Grants</t>
+  </si>
+  <si>
+    <t>Loans</t>
+  </si>
+  <si>
+    <t>Aggregate Awards</t>
+  </si>
+  <si>
+    <t>Aggregate Individuals</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Congressional District</t>
+  </si>
+  <si>
+    <t>RI Other Expenditure Categories</t>
+  </si>
+  <si>
+    <t>Is Awardee Complying with Terms and Conditions of the Grant?</t>
+  </si>
+  <si>
+    <t>Dropdown Options</t>
+  </si>
+  <si>
+    <t>State Government</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Purchase Order</t>
+  </si>
+  <si>
+    <t>Healthy/Safe Government Facilities</t>
+  </si>
+  <si>
+    <t>Lump Sum Payment(s)</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Less than 50% completed</t>
+  </si>
+  <si>
+    <t>County Government</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
+    <t>Delivery Order</t>
+  </si>
+  <si>
+    <t>tbd</t>
+  </si>
+  <si>
+    <t>Reimbursable</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>No, Returning to Treasury</t>
+  </si>
+  <si>
+    <t>Completed 50% or more</t>
+  </si>
+  <si>
+    <t>City or Township Government</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>MEX</t>
+  </si>
+  <si>
+    <t>Blanket Purchase Agreement</t>
+  </si>
+  <si>
+    <t>Fully completed</t>
+  </si>
+  <si>
+    <t>Special District Government</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>Definitive Contract</t>
+  </si>
+  <si>
+    <t>Transfers</t>
+  </si>
+  <si>
+    <t>Regional Organization</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>Direct Payments</t>
+  </si>
+  <si>
+    <t>U.S. Territory or Possession</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Independent School District</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>Public/State Controlled Institution of Higher Education</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>Indian/Native American Tribal Government (Federally Recognized)</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>Indian/Native American Tribal Government (Other than Federally Recognized)</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>Indian/Native American Tribal Designated Organization</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>Public/Indian Housing Authority</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>Nonprofit with 501C3 IRS Status (Other than IHE)</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>Nonprofit without 501C3 IRS Status (Other than IHE)</t>
+  </si>
+  <si>
+    <t>GU</t>
+  </si>
+  <si>
+    <t>Private Institution of Higher Education</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>For-Profit Organization (Other than Small Business)</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>Small Business</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>Hispanic-serving Institution</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>Historically Black College or University (HBCU)</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>Tribally Controlled College or University (TCCU)</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>Alaska Native and Native Hawaiian Serving Institutions</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>Non-domestic (non-U.S.) Entity</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>MH</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>PW</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
 </sst>
 </file>
 
@@ -385,7 +743,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -465,8 +823,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,8 +856,20 @@
         <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9CB9C"/>
+        <bgColor rgb="FFF9CB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE599"/>
+        <bgColor rgb="FFFFE599"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -515,13 +892,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -584,11 +971,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{11D4221D-0DF3-D04D-83B1-E1C09A364542}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{2FCA0F19-FEBD-3F44-BD57-8ECC545AD3DF}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -4921,6 +5316,606 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2403EBF0-B18D-FC40-9C8A-3EB4D7D2F8C5}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:Z61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="2" width="14.5" style="31"/>
+    <col min="3" max="3" width="57" style="31" customWidth="1"/>
+    <col min="4" max="16384" width="14.5" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+    </row>
+    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30"/>
+    </row>
+    <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" s="33">
+        <v>1</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="K3" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="L3" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="M3" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="N3" s="33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" s="33">
+        <v>2</v>
+      </c>
+      <c r="H4" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="K4" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="L4" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="M4" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="N4" s="33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>229</v>
+      </c>
+      <c r="L5" s="33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="L6" s="33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="L7" s="33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" s="36"/>
+    </row>
+    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D27" s="33" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="34"/>
+      <c r="D28" s="33" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D29" s="33" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D30" s="33" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D31" s="33" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D32" s="33" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D33" s="33" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D34" s="33" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D35" s="33" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D36" s="33" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D37" s="33" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D38" s="33" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D39" s="33" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D40" s="33" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D41" s="33" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D42" s="33" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D43" s="33" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D44" s="33" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D45" s="33" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D46" s="33" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D47" s="33" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D48" s="33" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D49" s="33" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D50" s="33" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D51" s="33" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D52" s="33" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D53" s="33" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D54" s="33" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D55" s="33" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D56" s="33" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D57" s="33" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="58" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D58" s="33" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D59" s="33" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="60" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D60" s="33" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="61" spans="4:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="D61" s="33" t="s">
+        <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA1"/>
@@ -5095,7 +6090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AX1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>